<commit_message>
put run simulation button after IO
</commit_message>
<xml_diff>
--- a/main_streamlit_v3_temp.xlsx
+++ b/main_streamlit_v3_temp.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>33478.81506678486</v>
+        <v>33452.02960683603</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>33420.90928419799</v>
+        <v>33416.04744270352</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>33435.44136801924</v>
+        <v>33428.64858119172</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>33333.65047310324</v>
+        <v>33334.21667591591</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>33118.42276000287</v>
+        <v>33184.44809034982</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>32966.91840849206</v>
+        <v>32975.84078225301</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>33009.48841747743</v>
+        <v>33011.55169400804</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>33013.97205489104</v>
+        <v>32975.13320882477</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>32792.28219869739</v>
+        <v>32805.19348058276</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>32589.78314828302</v>
+        <v>32634.48512479875</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>32502.5185234276</v>
+        <v>32508.79416243713</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>32480.46586535659</v>
+        <v>32482.02259935138</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>32495.1668163725</v>
+        <v>32510.15110191844</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>32357.10701789552</v>
+        <v>32309.01164024487</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>32222.38041966104</v>
+        <v>32303.57034460452</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>32371.38677494133</v>
+        <v>32368.46900602943</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>32408.16229372749</v>
+        <v>32424.29800875598</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>32292.4914392446</v>
+        <v>32289.62553800494</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>32242.33427867746</v>
+        <v>32200.02935571772</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>32195.31454491887</v>
+        <v>32242.01235459997</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>32301.41850730323</v>
+        <v>32351.16323853311</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>32011.81235460468</v>
+        <v>32105.96981491959</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>32009.82951749931</v>
+        <v>31943.94469998771</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>32068.92081806821</v>
+        <v>32073.11814260486</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>32133.12771012427</v>
+        <v>32154.88694852356</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>32189.80687582662</v>
+        <v>32208.2683725684</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>31876.27764076117</v>
+        <v>31908.54353754226</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>30888.40991275329</v>
+        <v>30642.85604881407</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>31073.72217334309</v>
+        <v>31068.17665796504</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>31028.87723212353</v>
+        <v>31008.83988945493</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>30733.16914335431</v>
+        <v>30734.55695843923</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>30526.23941999391</v>
+        <v>30611.35030012325</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>30831.00181577364</v>
+        <v>30799.50791153299</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>30990.34446200331</v>
+        <v>30967.59615007453</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>30941.24452214186</v>
+        <v>30873.29989747982</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>30759.48917106709</v>
+        <v>30796.53690408655</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>30939.43222481702</v>
+        <v>30551.13515675055</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>30575.85548093979</v>
+        <v>30575.81542639952</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>30575.85548093979</v>
+        <v>30572.6086179704</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>30503.17193642068</v>
+        <v>30547.83795904304</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>30471.48446966815</v>
+        <v>30471.44441512788</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>30470.71769005277</v>
+        <v>30470.6776355125</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>30467.46744601246</v>
+        <v>30356.83820936358</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>30231.6697955068</v>
+        <v>30213.1546442889</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>30217.7662959661</v>
+        <v>30212.38023607982</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>30295.85654773215</v>
+        <v>30297.98927386082</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>30400.26031829821</v>
+        <v>30385.26081484321</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>30503.03417338099</v>
+        <v>30467.13777328087</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>30303.90781878912</v>
+        <v>30319.03494357815</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>29718.67058278512</v>
+        <v>29686.55449616881</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>29819.4777895396</v>
+        <v>29756.91414088169</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>29881.85449947708</v>
+        <v>29839.04640216875</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>29827.02057623355</v>
+        <v>29820.55082688458</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>29703.21335150688</v>
+        <v>29649.71324350654</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>29802.0761716879</v>
+        <v>29743.23005834155</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>29906.03514012962</v>
+        <v>29841.84302143726</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>29776.97186613633</v>
+        <v>29596.19076996803</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>29523.2619840217</v>
+        <v>29450.81339309886</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>29623.42142748027</v>
+        <v>29543.19129274989</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>29712.91235381294</v>
+        <v>29634.8434108577</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>29409.44309308446</v>
+        <v>29219.29997703242</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>29062.84376215855</v>
+        <v>28966.57561139015</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>29167.2255075402</v>
+        <v>29057.33278001472</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>29252.34204593384</v>
+        <v>29145.38188447343</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>29357.20101258246</v>
+        <v>29246.95598604753</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>29053.11860278174</v>
+        <v>28993.89488688272</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>28805.68196491533</v>
+        <v>28681.97790506395</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>28898.26280808435</v>
+        <v>28771.36731105049</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>28979.10212193799</v>
+        <v>28864.64162605524</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>28595.91481058921</v>
+        <v>28458.24801734745</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>28251.26572679233</v>
+        <v>28106.88352790985</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>28322.00089065661</v>
+        <v>28162.76178356502</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>28416.69815806203</v>
+        <v>28264.33588513912</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>27818.86542077088</v>
+        <v>27622.83676622821</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>27370.47678091495</v>
+        <v>27205.37591407311</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>27446.53332665482</v>
+        <v>27264.59249876102</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>27520.93577219608</v>
+        <v>27344.47754123756</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>27603.78166506093</v>
+        <v>27444.4684550722</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>27128.69824966326</v>
+        <v>27035.47954344309</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>26780.88299123914</v>
+        <v>26610.90267570942</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>26883.28134524274</v>
+        <v>26622.94960653624</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>26912.92355155635</v>
+        <v>26711.35061974639</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>26625.21091182594</v>
+        <v>26400.83758162509</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>26186.28391665861</v>
+        <v>25972.40364827805</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>26257.71999498324</v>
+        <v>26022.68150651307</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>26321.45773556408</v>
+        <v>26098.74984110688</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>26298.04665086719</v>
+        <v>25856.61943233096</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>25908.83163835726</v>
+        <v>25662.97805429606</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>25699.18979711265</v>
+        <v>25454.77825319822</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>25794.66903855914</v>
+        <v>25549.58160348714</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>25895.37536983822</v>
+        <v>25646.26474413522</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>25964.82320751908</v>
+        <v>25737.63981494185</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>26064.62843546727</v>
+        <v>25802.63411897263</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>26108.3892288073</v>
+        <v>25841.04890696665</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>26215.3093357274</v>
+        <v>25942.62300854076</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>26154.40647590633</v>
+        <v>25934.18438418673</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>26139.19937246746</v>
+        <v>25852.89319805034</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>26243.19164284911</v>
+        <v>25948.64422270136</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>26339.99549335897</v>
+        <v>26045.92514478829</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>26446.91560027907</v>
+        <v>26147.49924636239</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>26459.74769946282</v>
+        <v>26027.0704228528</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>26374.58950335758</v>
+        <v>26064.52119328914</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>26481.50961027769</v>
+        <v>26166.09529486324</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>26580.57042192233</v>
+        <v>26259.81010116188</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>26628.83344915717</v>
+        <v>26302.85011935838</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>26337.21250681176</v>
+        <v>26005.76017535929</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>26444.13261373187</v>
+        <v>26107.33427693339</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>26551.05272065198</v>
+        <v>26208.90837850749</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>26418.62116818142</v>
+        <v>26179.04562046386</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>26324.95814330761</v>
+        <v>25989.09310025768</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>26422.07270649195</v>
+        <v>26071.64056190167</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>26528.99281341206</v>
+        <v>26165.46444988354</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>26495.10441562832</v>
+        <v>26127.18647393826</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>26466.14591132028</v>
+        <v>26121.62757055038</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>26429.78821560437</v>
+        <v>26050.22183603783</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>26533.36437347989</v>
+        <v>26148.45198856734</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>26640.2844804</v>
+        <v>26250.02609014144</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>26627.46291268963</v>
+        <v>26204.22692825878</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>26503.34796936424</v>
+        <v>26102.39756841367</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>26608.77353655832</v>
+        <v>26202.47713026175</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>26707.72181254116</v>
+        <v>26296.07940089858</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>26417.24525080292</v>
+        <v>26008.99881118023</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>26340.06199335467</v>
+        <v>25890.17297842748</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>26405.83527467248</v>
+        <v>25978.15484699187</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>26511.79347867996</v>
+        <v>26078.76704565335</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>26596.90014970264</v>
+        <v>26158.52771133001</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>26349.3039185534</v>
+        <v>25988.51922817296</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>25046.22773743668</v>
+        <v>24597.16328837206</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>25141.03752270074</v>
+        <v>24692.4545682901</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>25247.95762962085</v>
+        <v>24788.20116986421</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>25132.82379621352</v>
+        <v>24505.99523804776</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>23957.25768593326</v>
+        <v>23489.87557854199</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>24063.23236977645</v>
+        <v>23587.36316171896</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>24143.30220531887</v>
+        <v>23667.28162226742</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>23912.24652557166</v>
+        <v>23411.50229448806</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>23679.39292064699</v>
+        <v>23185.90689035285</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>23738.34262265564</v>
+        <v>23242.00039397286</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>23834.6117615862</v>
+        <v>23280.9014151942</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>23858.23731402117</v>
+        <v>23350.36680615055</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>23867.60608154373</v>
+        <v>23348.83670219993</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>23869.47812274478</v>
+        <v>23350.91560418215</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>23966.7917073719</v>
+        <v>23442.88318346325</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>24073.711814292</v>
+        <v>23544.45728503736</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>24171.09131223775</v>
+        <v>23635.01414302171</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>24267.2564569201</v>
+        <v>23727.30991697343</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>24374.17656384021</v>
+        <v>23828.88401854753</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>24481.09667076031</v>
+        <v>23930.45812012163</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>24533.60971032071</v>
+        <v>23756.50599891226</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>24100.23533750883</v>
+        <v>23538.90477617816</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>24207.15544442894</v>
+        <v>23640.47887775226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>